<commit_message>
view section&progress increase added
</commit_message>
<xml_diff>
--- a/DBData.xlsx
+++ b/DBData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e6ed007d93ab40d8/Atelerik/Git_code/poodle-e-learning-platform/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="11_AD4DF75460589B3ACB728457A79B58BA5BDEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BD1D8A0-1ED3-46AB-862B-395B458B092B}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="11_AD4DF75460589B3ACB728457A79B58BA5BDEDD8E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB86E46B-68A0-464A-BF3C-9AA74A88FEBC}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" tabRatio="838" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" tabRatio="838" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="courses" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="78">
   <si>
     <t>Core Python</t>
   </si>
@@ -187,6 +187,90 @@
   </si>
   <si>
     <t>77dc7699-4e3f-448a-9133-fb676d8b373b</t>
+  </si>
+  <si>
+    <t>users_id</t>
+  </si>
+  <si>
+    <t>courses_id</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>progress</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>verification_token</t>
+  </si>
+  <si>
+    <t>is_verified</t>
+  </si>
+  <si>
+    <t>is_approved</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>linked_in_account</t>
+  </si>
+  <si>
+    <t>expertise_area</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>external_link</t>
+  </si>
+  <si>
+    <t>tags_id</t>
+  </si>
+  <si>
+    <t>objectives_id</t>
+  </si>
+  <si>
+    <t>home_page_pic</t>
+  </si>
+  <si>
+    <t>owner_id</t>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>is_premium</t>
+  </si>
+  <si>
+    <t>course_rating</t>
   </si>
 </sst>
 </file>
@@ -245,6 +329,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -510,47 +598,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="12.19921875" customWidth="1"/>
+    <col min="4" max="4" width="13.73046875" customWidth="1"/>
+    <col min="7" max="7" width="10.265625" customWidth="1"/>
+    <col min="8" max="8" width="11.59765625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A1" s="1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1">
-        <v>0</v>
-      </c>
-      <c r="H1" s="1">
-        <v>8</v>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1">
@@ -560,21 +656,21 @@
         <v>1</v>
       </c>
       <c r="G2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="1">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1">
@@ -584,9 +680,33 @@
         <v>1</v>
       </c>
       <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H4" s="1">
         <v>7</v>
       </c>
     </row>
@@ -597,20 +717,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A7FA783-019B-4673-A14E-88C0BA6E3855}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.9296875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
@@ -618,14 +741,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
         <v>4</v>
       </c>
     </row>
@@ -636,25 +767,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B6D1229-DA54-495C-BDEA-C689135F68AE}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" s="1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -662,9 +793,17 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
     </row>
@@ -675,27 +814,38 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{264AB5C3-9535-4E24-888B-E62A183CD0B0}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="17" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -706,49 +856,52 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{100EC4D5-8D2C-4F90-8133-390F9522F4F3}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="37.3984375" customWidth="1"/>
+    <col min="4" max="4" width="14.59765625" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1">
-        <v>1</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>11</v>
@@ -759,16 +912,16 @@
     </row>
     <row r="3" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>11</v>
@@ -779,41 +932,61 @@
     </row>
     <row r="4" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="1">
         <v>2</v>
       </c>
     </row>
@@ -824,19 +997,30 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E08F309-615E-44C8-90ED-50262A3F82C8}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="15.46484375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A1" s="1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -847,25 +1031,37 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F151D19-1741-476A-B51C-E36606585CA9}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="33.3984375" customWidth="1"/>
+    <col min="3" max="3" width="32.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="57" x14ac:dyDescent="0.45">
-      <c r="A1" s="1">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="57" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
         <v>888345600</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -876,62 +1072,70 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1339D099-56B8-4BB6-B8BC-AFC7B895F248}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="5" max="5" width="12.46484375" customWidth="1"/>
+    <col min="6" max="6" width="17.19921875" customWidth="1"/>
+    <col min="8" max="8" width="15.9296875" customWidth="1"/>
+    <col min="10" max="10" width="12.06640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1">
-        <v>0</v>
-      </c>
-      <c r="J1" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="114" x14ac:dyDescent="0.45">
-      <c r="B2" s="1">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1">
@@ -941,88 +1145,115 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" ht="114" x14ac:dyDescent="0.45">
       <c r="B3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="114" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>44</v>
-      </c>
+      <c r="H4" s="1"/>
       <c r="I4" s="1">
         <v>1</v>
       </c>
       <c r="J4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="114" x14ac:dyDescent="0.45">
       <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="114" x14ac:dyDescent="0.45">
+      <c r="B6" s="1">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I6" s="1">
         <v>0</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J6" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1033,47 +1264,49 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0111E448-7C29-4F70-A096-9068DB58DF68}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="1">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1"/>
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
       </c>
       <c r="D2" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -1082,7 +1315,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -1091,7 +1324,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -1100,6 +1333,56 @@
         <v>7</v>
       </c>
       <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>7</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>